<commit_message>
Enhance dashboard functionality: hide ID column in members view, add forms for new member and event attendance, and improve point logging with validation warnings. Update save logic to preserve existing sheets in Excel workbook.
</commit_message>
<xml_diff>
--- a/data/members.xlsx
+++ b/data/members.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,15 +437,20 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>StudentID</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Points</t>
         </is>
@@ -453,132 +458,192 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
         <v>215317</v>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>Ana Reyes</t>
         </is>
       </c>
-      <c r="C2" t="n">
-        <v>128</v>
+      <c r="D2" t="n">
+        <v>120</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
         <v>224892</v>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>Ben Santos</t>
         </is>
       </c>
-      <c r="C3" t="n">
+      <c r="D3" t="n">
         <v>95</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
         <v>231045</v>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>Carla Dizon</t>
         </is>
       </c>
-      <c r="C4" t="n">
+      <c r="D4" t="n">
         <v>140</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
         <v>247631</v>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>David Cruz</t>
         </is>
       </c>
-      <c r="C5" t="n">
+      <c r="D5" t="n">
         <v>60</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n">
         <v>208456</v>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>Elena Tan</t>
         </is>
       </c>
-      <c r="C6" t="n">
+      <c r="D6" t="n">
         <v>110</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="n">
         <v>219073</v>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>Frank Lim</t>
         </is>
       </c>
-      <c r="C7" t="n">
+      <c r="D7" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="n">
         <v>225814</v>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>Grace Uy</t>
         </is>
       </c>
-      <c r="C8" t="n">
-        <v>160</v>
+      <c r="D8" t="n">
+        <v>155</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="n">
         <v>203729</v>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>Harold Go</t>
         </is>
       </c>
-      <c r="C9" t="n">
+      <c r="D9" t="n">
         <v>80</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="n">
         <v>244561</v>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>Iris Ponce</t>
         </is>
       </c>
-      <c r="C10" t="n">
+      <c r="D10" t="n">
         <v>125</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="n">
         <v>218340</v>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>Julius Ng</t>
         </is>
       </c>
-      <c r="C11" t="n">
+      <c r="D11" t="n">
         <v>45</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr"/>
+      <c r="B12" t="n">
+        <v>123145</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Trek II</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr"/>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>123146</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Trek III</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -592,7 +657,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -692,6 +757,56 @@
         <v>231045</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Mass</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>224892</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Mass</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>225814</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Mass</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>208456</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Mass</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>231045</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Mass</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>219073</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>